<commit_message>
Fix tests and remnants from renaming and refactoring
</commit_message>
<xml_diff>
--- a/emeScheme.xlsx
+++ b/emeScheme.xlsx
@@ -194,7 +194,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>DATA_v0.9.5</t>
+    <t>DATA emeScheme v0.9.5</t>
   </si>
   <si>
     <t>Experiment</t>
@@ -3994,7 +3994,7 @@
     <col min="4" max="4" width="13.6719" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.6719" style="6" customWidth="1"/>
     <col min="6" max="6" width="28.1719" style="6" customWidth="1"/>
-    <col min="7" max="7" width="20.8516" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.6562" style="6" customWidth="1"/>
     <col min="8" max="256" width="14.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>